<commit_message>
tests pass; added transfer factor vector to check standard report
</commit_message>
<xml_diff>
--- a/test/template_results/test_template_output.xlsx
+++ b/test/template_results/test_template_output.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
     <t>Number of Components:</t>
   </si>
@@ -124,6 +124,24 @@
   </si>
   <si>
     <t>Sheet Name: Unknown Sample 1 (3)</t>
+  </si>
+  <si>
+    <t>Transfer Factor Vector (wrt component 1):</t>
+  </si>
+  <si>
+    <t>Basis Component (N/A)</t>
+  </si>
+  <si>
+    <t>0.502 ± 0.014</t>
+  </si>
+  <si>
+    <t>0.515 ± 0.031</t>
+  </si>
+  <si>
+    <t>0.339 ± 0.013</t>
+  </si>
+  <si>
+    <t>2.059 ± 0.075</t>
   </si>
   <si>
     <t>Component Mass Ratio Matrix</t>
@@ -956,6 +974,26 @@
         <v>0.2</v>
       </c>
     </row>
+    <row r="5" spans="2:7">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="6" spans="2:7" dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
@@ -1119,13 +1157,13 @@
         <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
@@ -1142,19 +1180,19 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="M3" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="N3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:14" dyDescent="0.25">
@@ -1177,22 +1215,22 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="N4" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1200,19 +1238,19 @@
         <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="N5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:14" dyDescent="0.25">
@@ -1238,19 +1276,19 @@
         <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:14" dyDescent="0.25">
@@ -1276,19 +1314,19 @@
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="M7" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="N7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:14" dyDescent="0.25">
@@ -1482,13 +1520,13 @@
         <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
@@ -1505,19 +1543,19 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="M3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="N3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:14" dyDescent="0.25">
@@ -1540,22 +1578,22 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="N4" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1563,19 +1601,19 @@
         <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K5" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="M5" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="N5" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:14" dyDescent="0.25">
@@ -1601,19 +1639,19 @@
         <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="K6" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="M6" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="N6" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:14" dyDescent="0.25">
@@ -1639,19 +1677,19 @@
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="L7" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="M7" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="N7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:14" dyDescent="0.25">
@@ -1845,13 +1883,13 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="L2" t="s">
         <v>14</v>
@@ -1868,19 +1906,19 @@
         <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="K3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="L3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="M3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="N3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:14" dyDescent="0.25">
@@ -1903,22 +1941,22 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="L4" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="M4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="N4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1926,19 +1964,19 @@
         <v>14</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="L5" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="M5" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="N5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:14" dyDescent="0.25">
@@ -1964,19 +2002,19 @@
         <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="K6" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="L6" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="N6" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:14" dyDescent="0.25">
@@ -2002,19 +2040,19 @@
         <v>16</v>
       </c>
       <c r="J7" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="L7" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="M7" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="N7" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:14" dyDescent="0.25">

</xml_diff>

<commit_message>
Added mass ratio matrices for each sample/sample comparison to sample output, as well as extracted ratio matrix diagonal values + errors for ease of comparison across samples
</commit_message>
<xml_diff>
--- a/test/template_results/test_template_output.xlsx
+++ b/test/template_results/test_template_output.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="263">
   <si>
     <t>Number of Components:</t>
   </si>
@@ -147,6 +147,9 @@
     <t>Component Mass Ratio Matrix</t>
   </si>
   <si>
+    <t>my name 1/my name 1</t>
+  </si>
+  <si>
     <t>comp2 </t>
   </si>
   <si>
@@ -216,6 +219,252 @@
     <t>0.834 ± 0.067</t>
   </si>
   <si>
+    <t>Matrix Diagonal</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>my name 1/3</t>
+  </si>
+  <si>
+    <t>1.195 ± 0.016</t>
+  </si>
+  <si>
+    <t>0.241 ± 0.013</t>
+  </si>
+  <si>
+    <t>0.062 ± 0.0042</t>
+  </si>
+  <si>
+    <t>0.0815 ± 0.0048</t>
+  </si>
+  <si>
+    <t>0.0977 ± 0.0054</t>
+  </si>
+  <si>
+    <t>3.53 ± 0.17</t>
+  </si>
+  <si>
+    <t>0.712 ± 0.04</t>
+  </si>
+  <si>
+    <t>0.183 ± 0.015</t>
+  </si>
+  <si>
+    <t>0.241 ± 0.018</t>
+  </si>
+  <si>
+    <t>0.289 ± 0.021</t>
+  </si>
+  <si>
+    <t>13.7 ± 1.0</t>
+  </si>
+  <si>
+    <t>2.77 ± 0.25</t>
+  </si>
+  <si>
+    <t>0.711 ± 0.038</t>
+  </si>
+  <si>
+    <t>0.936 ± 0.089</t>
+  </si>
+  <si>
+    <t>1.12 ± 0.1</t>
+  </si>
+  <si>
+    <t>10.39 ± 0.6</t>
+  </si>
+  <si>
+    <t>2.1 ± 0.16</t>
+  </si>
+  <si>
+    <t>0.539 ± 0.047</t>
+  </si>
+  <si>
+    <t>0.709 ± 0.043</t>
+  </si>
+  <si>
+    <t>0.849 ± 0.067</t>
+  </si>
+  <si>
+    <t>8.75 ± 0.5</t>
+  </si>
+  <si>
+    <t>1.77 ± 0.14</t>
+  </si>
+  <si>
+    <t>0.454 ± 0.04</t>
+  </si>
+  <si>
+    <t>0.597 ± 0.048</t>
+  </si>
+  <si>
+    <t>0.716 ± 0.042</t>
+  </si>
+  <si>
+    <t>my name 1/test 3</t>
+  </si>
+  <si>
+    <t>1.07 ± 0.012</t>
+  </si>
+  <si>
+    <t>0.216 ± 0.011</t>
+  </si>
+  <si>
+    <t>0.0555 ± 0.0037</t>
+  </si>
+  <si>
+    <t>0.073 ± 0.0042</t>
+  </si>
+  <si>
+    <t>0.0875 ± 0.0048</t>
+  </si>
+  <si>
+    <t>4.25 ± 0.17</t>
+  </si>
+  <si>
+    <t>0.857 ± 0.042</t>
+  </si>
+  <si>
+    <t>0.22 ± 0.017</t>
+  </si>
+  <si>
+    <t>0.29 ± 0.02</t>
+  </si>
+  <si>
+    <t>0.348 ± 0.023</t>
+  </si>
+  <si>
+    <t>16.7 ± 1.3</t>
+  </si>
+  <si>
+    <t>3.37 ± 0.31</t>
+  </si>
+  <si>
+    <t>0.867 ± 0.05</t>
+  </si>
+  <si>
+    <t>1.14 ± 0.11</t>
+  </si>
+  <si>
+    <t>1.37 ± 0.13</t>
+  </si>
+  <si>
+    <t>12.66 ± 0.79</t>
+  </si>
+  <si>
+    <t>2.55 ± 0.2</t>
+  </si>
+  <si>
+    <t>0.657 ± 0.06</t>
+  </si>
+  <si>
+    <t>0.864 ± 0.056</t>
+  </si>
+  <si>
+    <t>1.035 ± 0.085</t>
+  </si>
+  <si>
+    <t>10.56 ± 0.73</t>
+  </si>
+  <si>
+    <t>2.13 ± 0.18</t>
+  </si>
+  <si>
+    <t>0.548 ± 0.052</t>
+  </si>
+  <si>
+    <t>0.72 ± 0.064</t>
+  </si>
+  <si>
+    <t>0.863 ± 0.061</t>
+  </si>
+  <si>
+    <t>3/my name 1</t>
+  </si>
+  <si>
+    <t>0.837 ± 0.011</t>
+  </si>
+  <si>
+    <t>0.283 ± 0.013</t>
+  </si>
+  <si>
+    <t>0.0729 ± 0.0055</t>
+  </si>
+  <si>
+    <t>0.0963 ± 0.0055</t>
+  </si>
+  <si>
+    <t>0.1143 ± 0.0066</t>
+  </si>
+  <si>
+    <t>4.15 ± 0.22</t>
+  </si>
+  <si>
+    <t>1.404 ± 0.079</t>
+  </si>
+  <si>
+    <t>0.361 ± 0.033</t>
+  </si>
+  <si>
+    <t>0.477 ± 0.037</t>
+  </si>
+  <si>
+    <t>0.566 ± 0.043</t>
+  </si>
+  <si>
+    <t>16.1 ± 1.1</t>
+  </si>
+  <si>
+    <t>5.46 ± 0.45</t>
+  </si>
+  <si>
+    <t>1.406 ± 0.075</t>
+  </si>
+  <si>
+    <t>1.86 ± 0.16</t>
+  </si>
+  <si>
+    <t>2.2 ± 0.19</t>
+  </si>
+  <si>
+    <t>12.27 ± 0.72</t>
+  </si>
+  <si>
+    <t>4.15 ± 0.31</t>
+  </si>
+  <si>
+    <t>1.07 ± 0.1</t>
+  </si>
+  <si>
+    <t>1.411 ± 0.085</t>
+  </si>
+  <si>
+    <t>1.67 ± 0.14</t>
+  </si>
+  <si>
+    <t>10.24 ± 0.57</t>
+  </si>
+  <si>
+    <t>3.46 ± 0.25</t>
+  </si>
+  <si>
+    <t>0.892 ± 0.083</t>
+  </si>
+  <si>
+    <t>1.177 ± 0.093</t>
+  </si>
+  <si>
+    <t>1.397 ± 0.083</t>
+  </si>
+  <si>
+    <t>3/3</t>
+  </si>
+  <si>
     <t>0.338 ± 0.019</t>
   </si>
   <si>
@@ -277,6 +526,243 @@
   </si>
   <si>
     <t>0.843 ± 0.071</t>
+  </si>
+  <si>
+    <t>3/test 3</t>
+  </si>
+  <si>
+    <t>0.895 ± 0.012</t>
+  </si>
+  <si>
+    <t>0.303 ± 0.015</t>
+  </si>
+  <si>
+    <t>0.078 ± 0.0059</t>
+  </si>
+  <si>
+    <t>0.103 ± 0.006</t>
+  </si>
+  <si>
+    <t>0.1222 ± 0.007</t>
+  </si>
+  <si>
+    <t>3.56 ± 0.15</t>
+  </si>
+  <si>
+    <t>1.203 ± 0.056</t>
+  </si>
+  <si>
+    <t>0.31 ± 0.027</t>
+  </si>
+  <si>
+    <t>0.409 ± 0.029</t>
+  </si>
+  <si>
+    <t>0.486 ± 0.034</t>
+  </si>
+  <si>
+    <t>14.0 ± 1.1</t>
+  </si>
+  <si>
+    <t>4.73 ± 0.44</t>
+  </si>
+  <si>
+    <t>1.219 ± 0.084</t>
+  </si>
+  <si>
+    <t>1.61 ± 0.16</t>
+  </si>
+  <si>
+    <t>1.91 ± 0.19</t>
+  </si>
+  <si>
+    <t>10.6 ± 0.67</t>
+  </si>
+  <si>
+    <t>3.58 ± 0.28</t>
+  </si>
+  <si>
+    <t>0.923 ± 0.091</t>
+  </si>
+  <si>
+    <t>1.219 ± 0.08</t>
+  </si>
+  <si>
+    <t>1.45 ± 0.12</t>
+  </si>
+  <si>
+    <t>8.84 ± 0.62</t>
+  </si>
+  <si>
+    <t>2.99 ± 0.25</t>
+  </si>
+  <si>
+    <t>0.77 ± 0.079</t>
+  </si>
+  <si>
+    <t>1.017 ± 0.091</t>
+  </si>
+  <si>
+    <t>1.206 ± 0.088</t>
+  </si>
+  <si>
+    <t>test 3/my name 1</t>
+  </si>
+  <si>
+    <t>0.935 ± 0.01</t>
+  </si>
+  <si>
+    <t>0.2353 ± 0.0093</t>
+  </si>
+  <si>
+    <t>0.0598 ± 0.0047</t>
+  </si>
+  <si>
+    <t>0.079 ± 0.0049</t>
+  </si>
+  <si>
+    <t>0.0947 ± 0.0065</t>
+  </si>
+  <si>
+    <t>4.63 ± 0.24</t>
+  </si>
+  <si>
+    <t>1.166 ± 0.058</t>
+  </si>
+  <si>
+    <t>0.297 ± 0.028</t>
+  </si>
+  <si>
+    <t>0.392 ± 0.031</t>
+  </si>
+  <si>
+    <t>0.47 ± 0.04</t>
+  </si>
+  <si>
+    <t>18.0 ± 1.2</t>
+  </si>
+  <si>
+    <t>4.54 ± 0.35</t>
+  </si>
+  <si>
+    <t>1.153 ± 0.066</t>
+  </si>
+  <si>
+    <t>1.52 ± 0.14</t>
+  </si>
+  <si>
+    <t>1.83 ± 0.17</t>
+  </si>
+  <si>
+    <t>13.7 ± 0.79</t>
+  </si>
+  <si>
+    <t>3.45 ± 0.24</t>
+  </si>
+  <si>
+    <t>0.877 ± 0.085</t>
+  </si>
+  <si>
+    <t>1.158 ± 0.075</t>
+  </si>
+  <si>
+    <t>1.39 ± 0.12</t>
+  </si>
+  <si>
+    <t>11.43 ± 0.62</t>
+  </si>
+  <si>
+    <t>2.88 ± 0.19</t>
+  </si>
+  <si>
+    <t>0.731 ± 0.07</t>
+  </si>
+  <si>
+    <t>0.966 ± 0.08</t>
+  </si>
+  <si>
+    <t>1.158 ± 0.081</t>
+  </si>
+  <si>
+    <t>test 3/3</t>
+  </si>
+  <si>
+    <t>1.117 ± 0.015</t>
+  </si>
+  <si>
+    <t>0.281 ± 0.012</t>
+  </si>
+  <si>
+    <t>0.0715 ± 0.0057</t>
+  </si>
+  <si>
+    <t>0.0944 ± 0.006</t>
+  </si>
+  <si>
+    <t>0.1132 ± 0.0079</t>
+  </si>
+  <si>
+    <t>3.3 ± 0.16</t>
+  </si>
+  <si>
+    <t>0.831 ± 0.039</t>
+  </si>
+  <si>
+    <t>0.211 ± 0.019</t>
+  </si>
+  <si>
+    <t>0.279 ± 0.022</t>
+  </si>
+  <si>
+    <t>0.335 ± 0.028</t>
+  </si>
+  <si>
+    <t>12.82 ± 0.98</t>
+  </si>
+  <si>
+    <t>3.23 ± 0.28</t>
+  </si>
+  <si>
+    <t>0.82 ± 0.056</t>
+  </si>
+  <si>
+    <t>1.08 ± 0.11</t>
+  </si>
+  <si>
+    <t>1.3 ± 0.13</t>
+  </si>
+  <si>
+    <t>9.71 ± 0.56</t>
+  </si>
+  <si>
+    <t>2.44 ± 0.17</t>
+  </si>
+  <si>
+    <t>0.621 ± 0.061</t>
+  </si>
+  <si>
+    <t>0.82 ± 0.054</t>
+  </si>
+  <si>
+    <t>0.984 ± 0.088</t>
+  </si>
+  <si>
+    <t>8.18 ± 0.47</t>
+  </si>
+  <si>
+    <t>2.06 ± 0.14</t>
+  </si>
+  <si>
+    <t>0.523 ± 0.051</t>
+  </si>
+  <si>
+    <t>0.691 ± 0.059</t>
+  </si>
+  <si>
+    <t>0.829 ± 0.061</t>
+  </si>
+  <si>
+    <t>test 3/test 3</t>
   </si>
   <si>
     <t>1.0 ± 1.5e-18</t>
@@ -1132,7 +1618,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A07878-647D-40C4-9C02-05C3899C7F4B}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6:G16"/>
@@ -1144,12 +1630,12 @@
     <col min="3" max="3" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" dyDescent="0.25">
+    <row r="1" spans="1:17" dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" dyDescent="0.25">
+    <row r="2" spans="1:17" dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1159,43 +1645,37 @@
       <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M3" t="s">
         <v>15</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1215,7 +1695,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
         <v>37</v>
@@ -1232,10 +1712,16 @@
       <c r="N4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="P4">
+        <v>1.0</v>
+      </c>
+      <c r="Q4">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="I5" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
         <v>38</v>
@@ -1244,7 +1730,7 @@
         <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="M5" t="s">
         <v>52</v>
@@ -1252,8 +1738,14 @@
       <c r="N5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" dyDescent="0.25">
+      <c r="P5">
+        <v>1.0</v>
+      </c>
+      <c r="Q5">
+        <v>7.39281446747491e-18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1273,7 +1765,7 @@
         <v>0.19400000000000001</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
         <v>39</v>
@@ -1282,16 +1774,22 @@
         <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="N6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" dyDescent="0.25">
+      <c r="P6">
+        <v>1.0</v>
+      </c>
+      <c r="Q6">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1311,7 +1809,7 @@
         <v>0.192</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
         <v>40</v>
@@ -1323,13 +1821,19 @@
         <v>49</v>
       </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="N7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="P7">
+        <v>1.0</v>
+      </c>
+      <c r="Q7">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -1348,8 +1852,32 @@
       <c r="G8">
         <v>0.19800000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8">
+        <v>1.0</v>
+      </c>
+      <c r="Q8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1369,7 +1897,7 @@
         <v>0.20600000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:14" dyDescent="0.25">
+    <row r="10" spans="1:17" dyDescent="0.25">
       <c r="C10">
         <v>4.95</v>
       </c>
@@ -1386,7 +1914,7 @@
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:14" dyDescent="0.25">
+    <row r="11" spans="1:17" dyDescent="0.25">
       <c r="C11">
         <v>4.8</v>
       </c>
@@ -1402,8 +1930,14 @@
       <c r="G11">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" dyDescent="0.25">
       <c r="C12">
         <v>4.75</v>
       </c>
@@ -1419,8 +1953,32 @@
       <c r="G12">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" dyDescent="0.25">
       <c r="C13">
         <v>5</v>
       </c>
@@ -1436,8 +1994,32 @@
       <c r="G13">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L13" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" t="s">
+        <v>78</v>
+      </c>
+      <c r="N13" t="s">
+        <v>83</v>
+      </c>
+      <c r="P13">
+        <v>1.194762947148681</v>
+      </c>
+      <c r="Q13">
+        <v>0.016288935342699585</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" dyDescent="0.25">
       <c r="C14">
         <v>5.15</v>
       </c>
@@ -1453,8 +2035,32 @@
       <c r="G14">
         <v>0.192</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" t="s">
+        <v>74</v>
+      </c>
+      <c r="M14" t="s">
+        <v>79</v>
+      </c>
+      <c r="N14" t="s">
+        <v>84</v>
+      </c>
+      <c r="P14">
+        <v>0.7124079667328213</v>
+      </c>
+      <c r="Q14">
+        <v>0.04016534927208739</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" dyDescent="0.25">
       <c r="C15">
         <v>5</v>
       </c>
@@ -1470,8 +2076,32 @@
       <c r="G15">
         <v>0.20800000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" t="s">
+        <v>80</v>
+      </c>
+      <c r="N15" t="s">
+        <v>85</v>
+      </c>
+      <c r="P15">
+        <v>0.7114852860926769</v>
+      </c>
+      <c r="Q15">
+        <v>0.03821391409446688</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" dyDescent="0.25">
       <c r="C16">
         <v>5.05</v>
       </c>
@@ -1486,6 +2116,220 @@
       </c>
       <c r="G16">
         <v>0.19800000000000001</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>66</v>
+      </c>
+      <c r="K16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L16" t="s">
+        <v>76</v>
+      </c>
+      <c r="M16" t="s">
+        <v>81</v>
+      </c>
+      <c r="N16" t="s">
+        <v>86</v>
+      </c>
+      <c r="P16">
+        <v>0.7085683077009126</v>
+      </c>
+      <c r="Q16">
+        <v>0.04260950608799644</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" t="s">
+        <v>72</v>
+      </c>
+      <c r="L17" t="s">
+        <v>77</v>
+      </c>
+      <c r="M17" t="s">
+        <v>82</v>
+      </c>
+      <c r="N17" t="s">
+        <v>87</v>
+      </c>
+      <c r="P17">
+        <v>0.7156476061369028</v>
+      </c>
+      <c r="Q17">
+        <v>0.0424642921765923</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+      <c r="P20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="I21" t="s">
+        <v>88</v>
+      </c>
+      <c r="J21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>89</v>
+      </c>
+      <c r="K22" t="s">
+        <v>94</v>
+      </c>
+      <c r="L22" t="s">
+        <v>99</v>
+      </c>
+      <c r="M22" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" t="s">
+        <v>109</v>
+      </c>
+      <c r="P22">
+        <v>1.0697753662140979</v>
+      </c>
+      <c r="Q22">
+        <v>0.01165882526197793</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" t="s">
+        <v>90</v>
+      </c>
+      <c r="K23" t="s">
+        <v>95</v>
+      </c>
+      <c r="L23" t="s">
+        <v>100</v>
+      </c>
+      <c r="M23" t="s">
+        <v>105</v>
+      </c>
+      <c r="N23" t="s">
+        <v>110</v>
+      </c>
+      <c r="P23">
+        <v>0.857277902743328</v>
+      </c>
+      <c r="Q23">
+        <v>0.042268568744109135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>91</v>
+      </c>
+      <c r="K24" t="s">
+        <v>96</v>
+      </c>
+      <c r="L24" t="s">
+        <v>101</v>
+      </c>
+      <c r="M24" t="s">
+        <v>106</v>
+      </c>
+      <c r="N24" t="s">
+        <v>111</v>
+      </c>
+      <c r="P24">
+        <v>0.8673288474942378</v>
+      </c>
+      <c r="Q24">
+        <v>0.049537102668832315</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" t="s">
+        <v>97</v>
+      </c>
+      <c r="L25" t="s">
+        <v>102</v>
+      </c>
+      <c r="M25" t="s">
+        <v>107</v>
+      </c>
+      <c r="N25" t="s">
+        <v>112</v>
+      </c>
+      <c r="P25">
+        <v>0.8637519307330512</v>
+      </c>
+      <c r="Q25">
+        <v>0.05585471860366028</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s">
+        <v>93</v>
+      </c>
+      <c r="K26" t="s">
+        <v>98</v>
+      </c>
+      <c r="L26" t="s">
+        <v>103</v>
+      </c>
+      <c r="M26" t="s">
+        <v>108</v>
+      </c>
+      <c r="N26" t="s">
+        <v>113</v>
+      </c>
+      <c r="P26">
+        <v>0.8633118796087639</v>
+      </c>
+      <c r="Q26">
+        <v>0.0607306014385384</v>
       </c>
     </row>
   </sheetData>
@@ -1495,7 +2339,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECB7571-8FB0-4DA8-8958-6D8775D9D74B}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6:G16"/>
@@ -1507,12 +2351,12 @@
     <col min="3" max="3" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" dyDescent="0.25">
+    <row r="1" spans="1:17" dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" dyDescent="0.25">
+    <row r="2" spans="1:17" dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1522,43 +2366,37 @@
       <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="I3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M3" t="s">
         <v>15</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" t="s">
-        <v>66</v>
-      </c>
-      <c r="M3" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1578,45 +2416,57 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="K4" t="s">
+        <v>120</v>
+      </c>
+      <c r="L4" t="s">
+        <v>125</v>
+      </c>
+      <c r="M4" t="s">
+        <v>130</v>
+      </c>
+      <c r="N4" t="s">
+        <v>135</v>
+      </c>
+      <c r="P4">
+        <v>0.836986117109268</v>
+      </c>
+      <c r="Q4">
+        <v>0.011411144593048237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="I5" t="s">
         <v>36</v>
       </c>
-      <c r="L4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
       <c r="J5" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="K5" t="s">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>126</v>
       </c>
       <c r="M5" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="N5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="P5">
+        <v>1.4036900858732761</v>
+      </c>
+      <c r="Q5">
+        <v>0.07913962954040196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1636,25 +2486,31 @@
         <v>0.192</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
       <c r="K6" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="M6" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="N6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="P6">
+        <v>1.405510443500221</v>
+      </c>
+      <c r="Q6">
+        <v>0.07549004371089314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1674,25 +2530,31 @@
         <v>0.19</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="L7" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="M7" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="N7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="P7">
+        <v>1.411296538571834</v>
+      </c>
+      <c r="Q7">
+        <v>0.08486782120888724</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -1711,8 +2573,32 @@
       <c r="G8">
         <v>0.20400000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K8" t="s">
+        <v>124</v>
+      </c>
+      <c r="L8" t="s">
+        <v>129</v>
+      </c>
+      <c r="M8" t="s">
+        <v>134</v>
+      </c>
+      <c r="N8" t="s">
+        <v>139</v>
+      </c>
+      <c r="P8">
+        <v>1.3973357717187707</v>
+      </c>
+      <c r="Q8">
+        <v>0.08291353729159102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -1732,7 +2618,7 @@
         <v>0.192</v>
       </c>
     </row>
-    <row r="10" spans="1:14" dyDescent="0.25">
+    <row r="10" spans="1:17" dyDescent="0.25">
       <c r="C10">
         <v>3</v>
       </c>
@@ -1749,7 +2635,7 @@
         <v>0.19400000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:14" dyDescent="0.25">
+    <row r="11" spans="1:17" dyDescent="0.25">
       <c r="C11">
         <v>2.9699999999999998</v>
       </c>
@@ -1765,8 +2651,14 @@
       <c r="G11">
         <v>0.20400000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" dyDescent="0.25">
       <c r="C12">
         <v>3.0300000000000002</v>
       </c>
@@ -1782,8 +2674,32 @@
       <c r="G12">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" dyDescent="0.25">
       <c r="C13">
         <v>2.8499999999999996</v>
       </c>
@@ -1799,8 +2715,32 @@
       <c r="G13">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" t="s">
+        <v>145</v>
+      </c>
+      <c r="L13" t="s">
+        <v>149</v>
+      </c>
+      <c r="M13" t="s">
+        <v>153</v>
+      </c>
+      <c r="N13" t="s">
+        <v>158</v>
+      </c>
+      <c r="P13">
+        <v>1.0</v>
+      </c>
+      <c r="Q13">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" dyDescent="0.25">
       <c r="C14">
         <v>2.8499999999999996</v>
       </c>
@@ -1816,8 +2756,32 @@
       <c r="G14">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>141</v>
+      </c>
+      <c r="K14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" t="s">
+        <v>150</v>
+      </c>
+      <c r="M14" t="s">
+        <v>154</v>
+      </c>
+      <c r="N14" t="s">
+        <v>159</v>
+      </c>
+      <c r="P14">
+        <v>1.0</v>
+      </c>
+      <c r="Q14">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" dyDescent="0.25">
       <c r="C15">
         <v>2.91</v>
       </c>
@@ -1833,8 +2797,32 @@
       <c r="G15">
         <v>0.20600000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>142</v>
+      </c>
+      <c r="K15" t="s">
+        <v>146</v>
+      </c>
+      <c r="L15" t="s">
+        <v>37</v>
+      </c>
+      <c r="M15" t="s">
+        <v>155</v>
+      </c>
+      <c r="N15" t="s">
+        <v>160</v>
+      </c>
+      <c r="P15">
+        <v>1.0</v>
+      </c>
+      <c r="Q15">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" dyDescent="0.25">
       <c r="C16">
         <v>3.0300000000000002</v>
       </c>
@@ -1849,6 +2837,220 @@
       </c>
       <c r="G16">
         <v>0.19800000000000001</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>143</v>
+      </c>
+      <c r="K16" t="s">
+        <v>147</v>
+      </c>
+      <c r="L16" t="s">
+        <v>151</v>
+      </c>
+      <c r="M16" t="s">
+        <v>156</v>
+      </c>
+      <c r="N16" t="s">
+        <v>161</v>
+      </c>
+      <c r="P16">
+        <v>1.0</v>
+      </c>
+      <c r="Q16">
+        <v>9.382980764784444e-18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>144</v>
+      </c>
+      <c r="K17" t="s">
+        <v>148</v>
+      </c>
+      <c r="L17" t="s">
+        <v>152</v>
+      </c>
+      <c r="M17" t="s">
+        <v>157</v>
+      </c>
+      <c r="N17" t="s">
+        <v>37</v>
+      </c>
+      <c r="P17">
+        <v>1.0</v>
+      </c>
+      <c r="Q17">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+      <c r="P20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="I21" t="s">
+        <v>162</v>
+      </c>
+      <c r="J21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>163</v>
+      </c>
+      <c r="K22" t="s">
+        <v>168</v>
+      </c>
+      <c r="L22" t="s">
+        <v>173</v>
+      </c>
+      <c r="M22" t="s">
+        <v>178</v>
+      </c>
+      <c r="N22" t="s">
+        <v>183</v>
+      </c>
+      <c r="P22">
+        <v>0.8953871299466829</v>
+      </c>
+      <c r="Q22">
+        <v>0.012116508803383146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" t="s">
+        <v>164</v>
+      </c>
+      <c r="K23" t="s">
+        <v>169</v>
+      </c>
+      <c r="L23" t="s">
+        <v>174</v>
+      </c>
+      <c r="M23" t="s">
+        <v>179</v>
+      </c>
+      <c r="N23" t="s">
+        <v>184</v>
+      </c>
+      <c r="P23">
+        <v>1.2033524929190442</v>
+      </c>
+      <c r="Q23">
+        <v>0.05645027879913091</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>165</v>
+      </c>
+      <c r="K24" t="s">
+        <v>170</v>
+      </c>
+      <c r="L24" t="s">
+        <v>175</v>
+      </c>
+      <c r="M24" t="s">
+        <v>180</v>
+      </c>
+      <c r="N24" t="s">
+        <v>185</v>
+      </c>
+      <c r="P24">
+        <v>1.2190397531021617</v>
+      </c>
+      <c r="Q24">
+        <v>0.08391681364713953</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" t="s">
+        <v>166</v>
+      </c>
+      <c r="K25" t="s">
+        <v>171</v>
+      </c>
+      <c r="L25" t="s">
+        <v>176</v>
+      </c>
+      <c r="M25" t="s">
+        <v>181</v>
+      </c>
+      <c r="N25" t="s">
+        <v>186</v>
+      </c>
+      <c r="P25">
+        <v>1.2190101100282935</v>
+      </c>
+      <c r="Q25">
+        <v>0.07955133667952484</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s">
+        <v>167</v>
+      </c>
+      <c r="K26" t="s">
+        <v>172</v>
+      </c>
+      <c r="L26" t="s">
+        <v>177</v>
+      </c>
+      <c r="M26" t="s">
+        <v>182</v>
+      </c>
+      <c r="N26" t="s">
+        <v>187</v>
+      </c>
+      <c r="P26">
+        <v>1.2063365715270946</v>
+      </c>
+      <c r="Q26">
+        <v>0.08831963005076039</v>
       </c>
     </row>
   </sheetData>
@@ -1858,7 +3060,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F52BBC26-209D-44A1-8D79-296EA416BDCE}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
@@ -1870,12 +3072,12 @@
     <col min="3" max="3" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" dyDescent="0.25">
+    <row r="1" spans="1:17" dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" dyDescent="0.25">
+    <row r="2" spans="1:17" dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -1885,43 +3087,37 @@
       <c r="I2" t="s">
         <v>34</v>
       </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="I3" t="s">
+        <v>188</v>
+      </c>
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M3" t="s">
         <v>15</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L3" t="s">
-        <v>88</v>
-      </c>
-      <c r="M3" t="s">
-        <v>93</v>
-      </c>
-      <c r="N3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -1941,45 +3137,57 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>80</v>
+        <v>189</v>
       </c>
       <c r="K4" t="s">
+        <v>194</v>
+      </c>
+      <c r="L4" t="s">
+        <v>199</v>
+      </c>
+      <c r="M4" t="s">
+        <v>204</v>
+      </c>
+      <c r="N4" t="s">
+        <v>209</v>
+      </c>
+      <c r="P4">
+        <v>0.9347756842999378</v>
+      </c>
+      <c r="Q4">
+        <v>0.01018754656967647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="I5" t="s">
         <v>36</v>
       </c>
-      <c r="L4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M4" t="s">
-        <v>94</v>
-      </c>
-      <c r="N4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
       <c r="J5" t="s">
-        <v>81</v>
+        <v>190</v>
       </c>
       <c r="K5" t="s">
-        <v>85</v>
+        <v>195</v>
       </c>
       <c r="L5" t="s">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="M5" t="s">
-        <v>95</v>
+        <v>205</v>
       </c>
       <c r="N5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="P5">
+        <v>1.1664828835549765</v>
+      </c>
+      <c r="Q5">
+        <v>0.057514094081499295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" dyDescent="0.25">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1999,25 +3207,31 @@
         <v>0.20400000000000001</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
-        <v>82</v>
+        <v>191</v>
       </c>
       <c r="K6" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
       <c r="L6" t="s">
-        <v>91</v>
+        <v>201</v>
       </c>
       <c r="M6" t="s">
-        <v>36</v>
+        <v>206</v>
       </c>
       <c r="N6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="P6">
+        <v>1.1529652252303801</v>
+      </c>
+      <c r="Q6">
+        <v>0.06585109777086039</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -2037,25 +3251,31 @@
         <v>0.19400000000000001</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>83</v>
+        <v>192</v>
       </c>
       <c r="K7" t="s">
-        <v>87</v>
+        <v>197</v>
       </c>
       <c r="L7" t="s">
-        <v>92</v>
+        <v>202</v>
       </c>
       <c r="M7" t="s">
-        <v>96</v>
+        <v>207</v>
       </c>
       <c r="N7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="P7">
+        <v>1.1577398144294941</v>
+      </c>
+      <c r="Q7">
+        <v>0.07486551317614192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" dyDescent="0.25">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -2074,8 +3294,32 @@
       <c r="G8">
         <v>0.20400000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" t="s">
+        <v>193</v>
+      </c>
+      <c r="K8" t="s">
+        <v>198</v>
+      </c>
+      <c r="L8" t="s">
+        <v>203</v>
+      </c>
+      <c r="M8" t="s">
+        <v>208</v>
+      </c>
+      <c r="N8" t="s">
+        <v>213</v>
+      </c>
+      <c r="P8">
+        <v>1.1583299426543052</v>
+      </c>
+      <c r="Q8">
+        <v>0.08148396395696898</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" dyDescent="0.25">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -2095,7 +3339,7 @@
         <v>0.20600000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:14" dyDescent="0.25">
+    <row r="10" spans="1:17" dyDescent="0.25">
       <c r="C10">
         <v>3.8</v>
       </c>
@@ -2112,7 +3356,7 @@
         <v>0.20400000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:14" dyDescent="0.25">
+    <row r="11" spans="1:17" dyDescent="0.25">
       <c r="C11">
         <v>4.16</v>
       </c>
@@ -2128,8 +3372,14 @@
       <c r="G11">
         <v>0.20200000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" dyDescent="0.25">
       <c r="C12">
         <v>3.84</v>
       </c>
@@ -2145,8 +3395,32 @@
       <c r="G12">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>214</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+      <c r="P12" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" dyDescent="0.25">
       <c r="C13">
         <v>4.2</v>
       </c>
@@ -2162,8 +3436,32 @@
       <c r="G13">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>215</v>
+      </c>
+      <c r="K13" t="s">
+        <v>220</v>
+      </c>
+      <c r="L13" t="s">
+        <v>225</v>
+      </c>
+      <c r="M13" t="s">
+        <v>230</v>
+      </c>
+      <c r="N13" t="s">
+        <v>235</v>
+      </c>
+      <c r="P13">
+        <v>1.1168353514971188</v>
+      </c>
+      <c r="Q13">
+        <v>0.015113178328964971</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" dyDescent="0.25">
       <c r="C14">
         <v>4.04</v>
       </c>
@@ -2179,8 +3477,32 @@
       <c r="G14">
         <v>0.192</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>36</v>
+      </c>
+      <c r="J14" t="s">
+        <v>216</v>
+      </c>
+      <c r="K14" t="s">
+        <v>221</v>
+      </c>
+      <c r="L14" t="s">
+        <v>226</v>
+      </c>
+      <c r="M14" t="s">
+        <v>231</v>
+      </c>
+      <c r="N14" t="s">
+        <v>236</v>
+      </c>
+      <c r="P14">
+        <v>0.8310116993020391</v>
+      </c>
+      <c r="Q14">
+        <v>0.03898345861830161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" dyDescent="0.25">
       <c r="C15">
         <v>4.16</v>
       </c>
@@ -2196,8 +3518,32 @@
       <c r="G15">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>217</v>
+      </c>
+      <c r="K15" t="s">
+        <v>222</v>
+      </c>
+      <c r="L15" t="s">
+        <v>227</v>
+      </c>
+      <c r="M15" t="s">
+        <v>232</v>
+      </c>
+      <c r="N15" t="s">
+        <v>237</v>
+      </c>
+      <c r="P15">
+        <v>0.8203177931279447</v>
+      </c>
+      <c r="Q15">
+        <v>0.05646940979748465</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" dyDescent="0.25">
       <c r="C16">
         <v>4.08</v>
       </c>
@@ -2212,6 +3558,220 @@
       </c>
       <c r="G16">
         <v>0.20600000000000002</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>218</v>
+      </c>
+      <c r="K16" t="s">
+        <v>223</v>
+      </c>
+      <c r="L16" t="s">
+        <v>228</v>
+      </c>
+      <c r="M16" t="s">
+        <v>233</v>
+      </c>
+      <c r="N16" t="s">
+        <v>238</v>
+      </c>
+      <c r="P16">
+        <v>0.8203377410682753</v>
+      </c>
+      <c r="Q16">
+        <v>0.053534390973286154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>219</v>
+      </c>
+      <c r="K17" t="s">
+        <v>224</v>
+      </c>
+      <c r="L17" t="s">
+        <v>229</v>
+      </c>
+      <c r="M17" t="s">
+        <v>234</v>
+      </c>
+      <c r="N17" t="s">
+        <v>239</v>
+      </c>
+      <c r="P17">
+        <v>0.8289560505772495</v>
+      </c>
+      <c r="Q17">
+        <v>0.060690435358883375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+      <c r="P20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="I21" t="s">
+        <v>240</v>
+      </c>
+      <c r="J21" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" t="s">
+        <v>36</v>
+      </c>
+      <c r="L21" t="s">
+        <v>14</v>
+      </c>
+      <c r="M21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N21" t="s">
+        <v>16</v>
+      </c>
+      <c r="P21" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="I22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" t="s">
+        <v>241</v>
+      </c>
+      <c r="K22" t="s">
+        <v>246</v>
+      </c>
+      <c r="L22" t="s">
+        <v>250</v>
+      </c>
+      <c r="M22" t="s">
+        <v>255</v>
+      </c>
+      <c r="N22" t="s">
+        <v>259</v>
+      </c>
+      <c r="P22">
+        <v>1.0</v>
+      </c>
+      <c r="Q22">
+        <v>1.511770898404307e-18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" t="s">
+        <v>242</v>
+      </c>
+      <c r="K23" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" t="s">
+        <v>251</v>
+      </c>
+      <c r="M23" t="s">
+        <v>256</v>
+      </c>
+      <c r="N23" t="s">
+        <v>260</v>
+      </c>
+      <c r="P23">
+        <v>1.0</v>
+      </c>
+      <c r="Q23">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>243</v>
+      </c>
+      <c r="K24" t="s">
+        <v>247</v>
+      </c>
+      <c r="L24" t="s">
+        <v>252</v>
+      </c>
+      <c r="M24" t="s">
+        <v>257</v>
+      </c>
+      <c r="N24" t="s">
+        <v>261</v>
+      </c>
+      <c r="P24">
+        <v>1.0</v>
+      </c>
+      <c r="Q24">
+        <v>1.3638636282673142e-17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" t="s">
+        <v>244</v>
+      </c>
+      <c r="K25" t="s">
+        <v>248</v>
+      </c>
+      <c r="L25" t="s">
+        <v>253</v>
+      </c>
+      <c r="M25" t="s">
+        <v>37</v>
+      </c>
+      <c r="N25" t="s">
+        <v>262</v>
+      </c>
+      <c r="P25">
+        <v>1.0</v>
+      </c>
+      <c r="Q25">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="I26" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" t="s">
+        <v>245</v>
+      </c>
+      <c r="K26" t="s">
+        <v>249</v>
+      </c>
+      <c r="L26" t="s">
+        <v>254</v>
+      </c>
+      <c r="M26" t="s">
+        <v>258</v>
+      </c>
+      <c r="N26" t="s">
+        <v>37</v>
+      </c>
+      <c r="P26">
+        <v>1.0</v>
+      </c>
+      <c r="Q26">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>